<commit_message>
added user by file
</commit_message>
<xml_diff>
--- a/src/img/Template.xlsx
+++ b/src/img/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osada\OneDrive\Desktop\final-dip\eyekondeploy\src\img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osada\OneDrive\Documents\Study\ondev\Work\wayo-live\src\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905F471F-765B-4103-B95C-2A8D9C5F67CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F3753B-4AA5-49AA-B46C-3ADBA0B519D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31395" yWindow="1365" windowWidth="17280" windowHeight="8970" xr2:uid="{359182AB-ACFC-40EB-93B6-7A6370A02C33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{359182AB-ACFC-40EB-93B6-7A6370A02C33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>students</t>
-  </si>
-  <si>
     <t>user name 1</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>user name 5</t>
+  </si>
+  <si>
+    <t>Audience Username</t>
   </si>
 </sst>
 </file>
@@ -418,9 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085161BD-6177-460F-B4A3-A94A7AC65A9B}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -429,32 +427,32 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>